<commit_message>
La Gaia ha pagato 100 €
</commit_message>
<xml_diff>
--- a/Netflix.xlsx
+++ b/Netflix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Netflix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADF0E172-48C6-4CAC-8CEC-F11CBBBB276D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C876676-C564-428D-B48F-DA44CA465726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,24 +18,11 @@
     <sheet name="Sheet 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="8">
   <si>
     <t>Rida</t>
   </si>
@@ -441,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -795,112 +782,86 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <f>ROUND(B8/B9,  1)</f>
-        <v>3.6</v>
-      </c>
-      <c r="C2" s="1">
-        <f t="shared" ref="C2:BN2" si="2">ROUND(C8/C9,  1)</f>
-        <v>3.6</v>
-      </c>
-      <c r="D2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="E2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="F2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="G2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="H2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="I2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="J2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="K2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="L2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="M2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="N2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="O2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="P2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="Q2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="R2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="S2" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-      <c r="T2" s="1">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="U2" s="1">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="V2" s="1">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="W2" s="1">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="X2" s="1">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="Y2" s="1">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="Z2" s="1">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="AA2" s="1">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>0.8</v>
       </c>
       <c r="AB2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C2:BN2" si="2">ROUND(AB8/AB9,  1)</f>
         <v>4.5</v>
       </c>
       <c r="AC2" s="1">
@@ -1798,335 +1759,335 @@
         <v>2022</v>
       </c>
       <c r="C5" s="1">
-        <f>IF(B1=12,B5+1,B5)</f>
+        <f t="shared" ref="C5:AH5" si="8">IF(B1=12,B5+1,B5)</f>
         <v>2022</v>
       </c>
       <c r="D5" s="1">
-        <f>IF(C1=12,C5+1,C5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="E5" s="1">
-        <f>IF(D1=12,D5+1,D5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="F5" s="1">
-        <f>IF(E1=12,E5+1,E5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="G5" s="1">
-        <f>IF(F1=12,F5+1,F5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="H5" s="1">
-        <f>IF(G1=12,G5+1,G5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="I5" s="1">
-        <f>IF(H1=12,H5+1,H5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="J5" s="1">
-        <f>IF(I1=12,I5+1,I5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="K5" s="1">
-        <f>IF(J1=12,J5+1,J5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="L5" s="1">
-        <f>IF(K1=12,K5+1,K5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="M5" s="1">
-        <f>IF(L1=12,L5+1,L5)</f>
+        <f t="shared" si="8"/>
         <v>2022</v>
       </c>
       <c r="N5" s="1">
-        <f>IF(M1=12,M5+1,M5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="O5" s="1">
-        <f>IF(N1=12,N5+1,N5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="P5" s="1">
-        <f>IF(O1=12,O5+1,O5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="Q5" s="1">
-        <f>IF(P1=12,P5+1,P5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="R5" s="1">
-        <f>IF(Q1=12,Q5+1,Q5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="S5" s="1">
-        <f>IF(R1=12,R5+1,R5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="T5" s="1">
-        <f>IF(S1=12,S5+1,S5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="U5" s="1">
-        <f>IF(T1=12,T5+1,T5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="V5" s="1">
-        <f>IF(U1=12,U5+1,U5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="W5" s="1">
-        <f>IF(V1=12,V5+1,V5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="X5" s="1">
-        <f>IF(W1=12,W5+1,W5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="Y5" s="1">
-        <f>IF(X1=12,X5+1,X5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="Z5" s="1">
-        <f>IF(Y1=12,Y5+1,Y5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AA5" s="1">
-        <f>IF(Z1=12,Z5+1,Z5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AB5" s="1">
-        <f>IF(AA1=12,AA5+1,AA5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AC5" s="1">
-        <f>IF(AB1=12,AB5+1,AB5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AD5" s="1">
-        <f>IF(AC1=12,AC5+1,AC5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AE5" s="1">
-        <f>IF(AD1=12,AD5+1,AD5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AF5" s="1">
-        <f>IF(AE1=12,AE5+1,AE5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AG5" s="1">
-        <f>IF(AF1=12,AF5+1,AF5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AH5" s="1">
-        <f>IF(AG1=12,AG5+1,AG5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="AI5" s="1">
-        <f>IF(AH1=12,AH5+1,AH5)</f>
+        <f t="shared" ref="AI5:BN5" si="9">IF(AH1=12,AH5+1,AH5)</f>
         <v>2024</v>
       </c>
       <c r="AJ5" s="1">
-        <f>IF(AI1=12,AI5+1,AI5)</f>
+        <f t="shared" si="9"/>
         <v>2024</v>
       </c>
       <c r="AK5" s="1">
-        <f>IF(AJ1=12,AJ5+1,AJ5)</f>
+        <f t="shared" si="9"/>
         <v>2024</v>
       </c>
       <c r="AL5" s="1">
-        <f>IF(AK1=12,AK5+1,AK5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AM5" s="1">
-        <f>IF(AL1=12,AL5+1,AL5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AN5" s="1">
-        <f>IF(AM1=12,AM5+1,AM5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AO5" s="1">
-        <f>IF(AN1=12,AN5+1,AN5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AP5" s="1">
-        <f>IF(AO1=12,AO5+1,AO5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AQ5" s="1">
-        <f>IF(AP1=12,AP5+1,AP5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AR5" s="1">
-        <f>IF(AQ1=12,AQ5+1,AQ5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AS5" s="1">
-        <f>IF(AR1=12,AR5+1,AR5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AT5" s="1">
-        <f>IF(AS1=12,AS5+1,AS5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AU5" s="1">
-        <f>IF(AT1=12,AT5+1,AT5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AV5" s="1">
-        <f>IF(AU1=12,AU5+1,AU5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AW5" s="1">
-        <f>IF(AV1=12,AV5+1,AV5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AX5" s="1">
-        <f>IF(AW1=12,AW5+1,AW5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AY5" s="1">
-        <f>IF(AX1=12,AX5+1,AX5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AZ5" s="1">
-        <f>IF(AY1=12,AY5+1,AY5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BA5" s="1">
-        <f>IF(AZ1=12,AZ5+1,AZ5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BB5" s="1">
-        <f>IF(BA1=12,BA5+1,BA5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BC5" s="1">
-        <f>IF(BB1=12,BB5+1,BB5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BD5" s="1">
-        <f>IF(BC1=12,BC5+1,BC5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BE5" s="1">
-        <f>IF(BD1=12,BD5+1,BD5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BF5" s="1">
-        <f>IF(BE1=12,BE5+1,BE5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BG5" s="1">
-        <f>IF(BF1=12,BF5+1,BF5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BH5" s="1">
-        <f>IF(BG1=12,BG5+1,BG5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BI5" s="1">
-        <f>IF(BH1=12,BH5+1,BH5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="BJ5" s="1">
-        <f>IF(BI1=12,BI5+1,BI5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BK5" s="1">
-        <f>IF(BJ1=12,BJ5+1,BJ5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BL5" s="1">
-        <f>IF(BK1=12,BK5+1,BK5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BM5" s="1">
-        <f>IF(BL1=12,BL5+1,BL5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BN5" s="1">
-        <f>IF(BM1=12,BM5+1,BM5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BO5" s="1">
-        <f>IF(BN1=12,BN5+1,BN5)</f>
+        <f t="shared" ref="BO5:CG5" si="10">IF(BN1=12,BN5+1,BN5)</f>
         <v>2027</v>
       </c>
       <c r="BP5" s="1">
-        <f>IF(BO1=12,BO5+1,BO5)</f>
+        <f t="shared" si="10"/>
         <v>2027</v>
       </c>
       <c r="BQ5" s="1">
-        <f>IF(BP1=12,BP5+1,BP5)</f>
+        <f t="shared" si="10"/>
         <v>2027</v>
       </c>
       <c r="BR5" s="1">
-        <f>IF(BQ1=12,BQ5+1,BQ5)</f>
+        <f t="shared" si="10"/>
         <v>2027</v>
       </c>
       <c r="BS5" s="1">
-        <f>IF(BR1=12,BR5+1,BR5)</f>
+        <f t="shared" si="10"/>
         <v>2027</v>
       </c>
       <c r="BT5" s="1">
-        <f>IF(BS1=12,BS5+1,BS5)</f>
+        <f t="shared" si="10"/>
         <v>2027</v>
       </c>
       <c r="BU5" s="1">
-        <f>IF(BT1=12,BT5+1,BT5)</f>
+        <f t="shared" si="10"/>
         <v>2027</v>
       </c>
       <c r="BV5" s="1">
-        <f>IF(BU1=12,BU5+1,BU5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BW5" s="1">
-        <f>IF(BV1=12,BV5+1,BV5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BX5" s="1">
-        <f>IF(BW1=12,BW5+1,BW5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BY5" s="1">
-        <f>IF(BX1=12,BX5+1,BX5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BZ5" s="1">
-        <f>IF(BY1=12,BY5+1,BY5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="CA5" s="1">
-        <f>IF(BZ1=12,BZ5+1,BZ5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="CB5" s="1">
-        <f>IF(CA1=12,CA5+1,CA5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="CC5" s="1">
-        <f>IF(CB1=12,CB5+1,CB5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="CD5" s="1">
-        <f>IF(CC1=12,CC5+1,CC5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="CE5" s="1">
-        <f>IF(CD1=12,CD5+1,CD5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="CF5" s="1">
-        <f>IF(CE1=12,CE5+1,CE5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="CG5" s="1">
-        <f>IF(CF1=12,CF5+1,CF5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rimosso il 2022 + .gitignore
</commit_message>
<xml_diff>
--- a/Netflix.xlsx
+++ b/Netflix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Netflix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C876676-C564-428D-B48F-DA44CA465726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1AEDC3-4171-4464-A89D-59B00C98DE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Rida</t>
   </si>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -821,72 +821,84 @@
       <c r="N2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>1</v>
+      <c r="O2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="P2" s="1">
+        <f t="shared" ref="P2:BB2" si="2">ROUND(AB8/AB9,  1)</f>
+        <v>4.5</v>
+      </c>
+      <c r="Q2" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="R2" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="S2" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="T2" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="U2" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="V2" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="W2" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="X2" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="Y2" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="Z2" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="AA2" s="1">
-        <v>0.8</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="AB2" s="1">
-        <f t="shared" ref="C2:BN2" si="2">ROUND(AB8/AB9,  1)</f>
-        <v>4.5</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="AC2" s="1">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AD2" s="1">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AE2" s="1">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AF2" s="1">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AG2" s="1">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AH2" s="1">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AI2" s="1">
         <f t="shared" si="2"/>
@@ -969,55 +981,55 @@
         <v>5</v>
       </c>
       <c r="BC2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="BC2:BU2" si="3">ROUND(BO8/BO9,  1)</f>
         <v>5</v>
       </c>
       <c r="BD2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BE2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BF2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BG2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BH2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BI2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BJ2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BK2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BL2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BM2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BN2" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BO2" s="1">
-        <f t="shared" ref="BO2:CG2" si="3">ROUND(BO8/BO9,  1)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BP2" s="1">
@@ -1041,54 +1053,6 @@
         <v>5</v>
       </c>
       <c r="BU2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="BV2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="BW2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="BX2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="BY2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="BZ2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="CA2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="CB2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="CC2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="CD2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="CE2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="CF2" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="CG2" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -1097,65 +1061,77 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="B3" s="1">
         <f>ROUND(N8/N9,  1)</f>
         <v>3.6</v>
       </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:BN3" si="4">ROUND(O8/O9,  1)</f>
+        <v>3.6</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="4"/>
+        <v>3.6</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="4"/>
+        <v>3.6</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="4"/>
+        <v>3.6</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="4"/>
+        <v>3.6</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
       <c r="O3" s="1">
-        <f t="shared" ref="O3:BZ3" si="4">ROUND(O8/O9,  1)</f>
-        <v>3.6</v>
+        <f t="shared" si="4"/>
+        <v>4.5</v>
       </c>
       <c r="P3" s="1">
         <f t="shared" si="4"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="Q3" s="1">
         <f t="shared" si="4"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="R3" s="1">
         <f t="shared" si="4"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="S3" s="1">
         <f t="shared" si="4"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="T3" s="1">
         <f t="shared" si="4"/>
@@ -1171,51 +1147,51 @@
       </c>
       <c r="W3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="X3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="Y3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AA3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AB3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AC3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AD3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AE3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AF3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AG3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AH3" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AI3" s="1">
         <f t="shared" si="4"/>
@@ -1346,78 +1322,30 @@
         <v>5</v>
       </c>
       <c r="BO3" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="BO3:BU3" si="5">ROUND(CA8/CA9,  1)</f>
         <v>5</v>
       </c>
       <c r="BP3" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BQ3" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BR3" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BS3" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BT3" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BU3" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="BV3" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="BW3" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="BX3" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="BY3" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="BZ3" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="CA3" s="1">
-        <f t="shared" ref="CA3:CG3" si="5">ROUND(CA8/CA9,  1)</f>
-        <v>5</v>
-      </c>
-      <c r="CB3" s="1">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="CC3" s="1">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="CD3" s="1">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="CE3" s="1">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="CF3" s="1">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="CG3" s="1">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
@@ -1426,65 +1354,77 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1">
+      <c r="B4" s="1">
         <f>ROUND(N8/N9,  1)</f>
         <v>3.6</v>
       </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:BN4" si="6">ROUND(O8/O9,  1)</f>
+        <v>3.6</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="6"/>
+        <v>3.6</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="6"/>
+        <v>3.6</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="6"/>
+        <v>3.6</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="6"/>
+        <v>3.6</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:BZ4" si="6">ROUND(O8/O9,  1)</f>
-        <v>3.6</v>
+        <f t="shared" si="6"/>
+        <v>4.5</v>
       </c>
       <c r="P4" s="1">
         <f t="shared" si="6"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" si="6"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="R4" s="1">
         <f t="shared" si="6"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="S4" s="1">
         <f t="shared" si="6"/>
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="T4" s="1">
         <f t="shared" si="6"/>
@@ -1500,51 +1440,51 @@
       </c>
       <c r="W4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="X4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="Y4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="Z4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AA4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AB4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AC4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AD4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AE4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AF4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AG4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AH4" s="1">
         <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="AI4" s="1">
         <f t="shared" si="6"/>
@@ -1675,78 +1615,30 @@
         <v>5</v>
       </c>
       <c r="BO4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="BO4:BU4" si="7">ROUND(CA8/CA9,  1)</f>
         <v>5</v>
       </c>
       <c r="BP4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BQ4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BR4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BS4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BT4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BU4" s="1">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="BV4" s="1">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="BW4" s="1">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="BX4" s="1">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="BY4" s="1">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="BZ4" s="1">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="CA4" s="1">
-        <f t="shared" ref="CA4:CG4" si="7">ROUND(CA8/CA9,  1)</f>
-        <v>5</v>
-      </c>
-      <c r="CB4" s="1">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="CC4" s="1">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="CD4" s="1">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="CE4" s="1">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="CF4" s="1">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="CG4" s="1">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
@@ -1756,338 +1648,290 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:AH5" si="8">IF(B1=12,B5+1,B5)</f>
-        <v>2022</v>
+        <f>IF(N1=12,B5+1,B5)</f>
+        <v>2023</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(O1=12,C5+1,C5)</f>
+        <v>2023</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(P1=12,D5+1,D5)</f>
+        <v>2023</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(Q1=12,E5+1,E5)</f>
+        <v>2023</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(R1=12,F5+1,F5)</f>
+        <v>2023</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(S1=12,G5+1,G5)</f>
+        <v>2023</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(T1=12,H5+1,H5)</f>
+        <v>2023</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(U1=12,I5+1,I5)</f>
+        <v>2023</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(V1=12,J5+1,J5)</f>
+        <v>2023</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(W1=12,K5+1,K5)</f>
+        <v>2023</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="8"/>
-        <v>2022</v>
+        <f>IF(X1=12,L5+1,L5)</f>
+        <v>2023</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(Y1=12,M5+1,M5)</f>
+        <v>2024</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(Z1=12,N5+1,N5)</f>
+        <v>2024</v>
       </c>
       <c r="P5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AA1=12,O5+1,O5)</f>
+        <v>2024</v>
       </c>
       <c r="Q5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AB1=12,P5+1,P5)</f>
+        <v>2024</v>
       </c>
       <c r="R5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AC1=12,Q5+1,Q5)</f>
+        <v>2024</v>
       </c>
       <c r="S5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AD1=12,R5+1,R5)</f>
+        <v>2024</v>
       </c>
       <c r="T5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AE1=12,S5+1,S5)</f>
+        <v>2024</v>
       </c>
       <c r="U5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AF1=12,T5+1,T5)</f>
+        <v>2024</v>
       </c>
       <c r="V5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AG1=12,U5+1,U5)</f>
+        <v>2024</v>
       </c>
       <c r="W5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AH1=12,V5+1,V5)</f>
+        <v>2024</v>
       </c>
       <c r="X5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AI1=12,W5+1,W5)</f>
+        <v>2024</v>
       </c>
       <c r="Y5" s="1">
-        <f t="shared" si="8"/>
-        <v>2023</v>
+        <f>IF(AJ1=12,X5+1,X5)</f>
+        <v>2024</v>
       </c>
       <c r="Z5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AK1=12,Y5+1,Y5)</f>
+        <v>2025</v>
       </c>
       <c r="AA5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AL1=12,Z5+1,Z5)</f>
+        <v>2025</v>
       </c>
       <c r="AB5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AM1=12,AA5+1,AA5)</f>
+        <v>2025</v>
       </c>
       <c r="AC5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AN1=12,AB5+1,AB5)</f>
+        <v>2025</v>
       </c>
       <c r="AD5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AO1=12,AC5+1,AC5)</f>
+        <v>2025</v>
       </c>
       <c r="AE5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AP1=12,AD5+1,AD5)</f>
+        <v>2025</v>
       </c>
       <c r="AF5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AQ1=12,AE5+1,AE5)</f>
+        <v>2025</v>
       </c>
       <c r="AG5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AR1=12,AF5+1,AF5)</f>
+        <v>2025</v>
       </c>
       <c r="AH5" s="1">
-        <f t="shared" si="8"/>
-        <v>2024</v>
+        <f>IF(AS1=12,AG5+1,AG5)</f>
+        <v>2025</v>
       </c>
       <c r="AI5" s="1">
-        <f t="shared" ref="AI5:BN5" si="9">IF(AH1=12,AH5+1,AH5)</f>
-        <v>2024</v>
+        <f>IF(AT1=12,AH5+1,AH5)</f>
+        <v>2025</v>
       </c>
       <c r="AJ5" s="1">
-        <f t="shared" si="9"/>
-        <v>2024</v>
+        <f>IF(AU1=12,AI5+1,AI5)</f>
+        <v>2025</v>
       </c>
       <c r="AK5" s="1">
-        <f t="shared" si="9"/>
-        <v>2024</v>
+        <f>IF(AV1=12,AJ5+1,AJ5)</f>
+        <v>2025</v>
       </c>
       <c r="AL5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(AW1=12,AK5+1,AK5)</f>
+        <v>2026</v>
       </c>
       <c r="AM5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(AX1=12,AL5+1,AL5)</f>
+        <v>2026</v>
       </c>
       <c r="AN5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(AY1=12,AM5+1,AM5)</f>
+        <v>2026</v>
       </c>
       <c r="AO5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(AZ1=12,AN5+1,AN5)</f>
+        <v>2026</v>
       </c>
       <c r="AP5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(BA1=12,AO5+1,AO5)</f>
+        <v>2026</v>
       </c>
       <c r="AQ5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(BB1=12,AP5+1,AP5)</f>
+        <v>2026</v>
       </c>
       <c r="AR5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(BC1=12,AQ5+1,AQ5)</f>
+        <v>2026</v>
       </c>
       <c r="AS5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(BD1=12,AR5+1,AR5)</f>
+        <v>2026</v>
       </c>
       <c r="AT5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(BE1=12,AS5+1,AS5)</f>
+        <v>2026</v>
       </c>
       <c r="AU5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(BF1=12,AT5+1,AT5)</f>
+        <v>2026</v>
       </c>
       <c r="AV5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(BG1=12,AU5+1,AU5)</f>
+        <v>2026</v>
       </c>
       <c r="AW5" s="1">
-        <f t="shared" si="9"/>
-        <v>2025</v>
+        <f>IF(BH1=12,AV5+1,AV5)</f>
+        <v>2026</v>
       </c>
       <c r="AX5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BI1=12,AW5+1,AW5)</f>
+        <v>2027</v>
       </c>
       <c r="AY5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BJ1=12,AX5+1,AX5)</f>
+        <v>2027</v>
       </c>
       <c r="AZ5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BK1=12,AY5+1,AY5)</f>
+        <v>2027</v>
       </c>
       <c r="BA5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BL1=12,AZ5+1,AZ5)</f>
+        <v>2027</v>
       </c>
       <c r="BB5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BM1=12,BA5+1,BA5)</f>
+        <v>2027</v>
       </c>
       <c r="BC5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BN1=12,BB5+1,BB5)</f>
+        <v>2027</v>
       </c>
       <c r="BD5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BO1=12,BC5+1,BC5)</f>
+        <v>2027</v>
       </c>
       <c r="BE5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BP1=12,BD5+1,BD5)</f>
+        <v>2027</v>
       </c>
       <c r="BF5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BQ1=12,BE5+1,BE5)</f>
+        <v>2027</v>
       </c>
       <c r="BG5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BR1=12,BF5+1,BF5)</f>
+        <v>2027</v>
       </c>
       <c r="BH5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BS1=12,BG5+1,BG5)</f>
+        <v>2027</v>
       </c>
       <c r="BI5" s="1">
-        <f t="shared" si="9"/>
-        <v>2026</v>
+        <f>IF(BT1=12,BH5+1,BH5)</f>
+        <v>2027</v>
       </c>
       <c r="BJ5" s="1">
-        <f t="shared" si="9"/>
-        <v>2027</v>
+        <f>IF(BU1=12,BI5+1,BI5)</f>
+        <v>2028</v>
       </c>
       <c r="BK5" s="1">
-        <f t="shared" si="9"/>
-        <v>2027</v>
+        <f>IF(BV1=12,BJ5+1,BJ5)</f>
+        <v>2028</v>
       </c>
       <c r="BL5" s="1">
-        <f t="shared" si="9"/>
-        <v>2027</v>
+        <f>IF(BW1=12,BK5+1,BK5)</f>
+        <v>2028</v>
       </c>
       <c r="BM5" s="1">
-        <f t="shared" si="9"/>
-        <v>2027</v>
+        <f>IF(BX1=12,BL5+1,BL5)</f>
+        <v>2028</v>
       </c>
       <c r="BN5" s="1">
-        <f t="shared" si="9"/>
-        <v>2027</v>
+        <f>IF(BY1=12,BM5+1,BM5)</f>
+        <v>2028</v>
       </c>
       <c r="BO5" s="1">
-        <f t="shared" ref="BO5:CG5" si="10">IF(BN1=12,BN5+1,BN5)</f>
-        <v>2027</v>
+        <f>IF(BZ1=12,BN5+1,BN5)</f>
+        <v>2028</v>
       </c>
       <c r="BP5" s="1">
-        <f t="shared" si="10"/>
-        <v>2027</v>
+        <f>IF(CA1=12,BO5+1,BO5)</f>
+        <v>2028</v>
       </c>
       <c r="BQ5" s="1">
-        <f t="shared" si="10"/>
-        <v>2027</v>
+        <f>IF(CB1=12,BP5+1,BP5)</f>
+        <v>2028</v>
       </c>
       <c r="BR5" s="1">
-        <f t="shared" si="10"/>
-        <v>2027</v>
+        <f>IF(CC1=12,BQ5+1,BQ5)</f>
+        <v>2028</v>
       </c>
       <c r="BS5" s="1">
-        <f t="shared" si="10"/>
-        <v>2027</v>
+        <f>IF(CD1=12,BR5+1,BR5)</f>
+        <v>2028</v>
       </c>
       <c r="BT5" s="1">
-        <f t="shared" si="10"/>
-        <v>2027</v>
+        <f>IF(CE1=12,BS5+1,BS5)</f>
+        <v>2028</v>
       </c>
       <c r="BU5" s="1">
-        <f t="shared" si="10"/>
-        <v>2027</v>
-      </c>
-      <c r="BV5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="BW5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="BX5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="BY5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="BZ5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="CA5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="CB5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="CC5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="CD5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="CE5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="CF5" s="1">
-        <f t="shared" si="10"/>
-        <v>2028</v>
-      </c>
-      <c r="CG5" s="1">
-        <f t="shared" si="10"/>
+        <f>IF(CF1=12,BT5+1,BT5)</f>
         <v>2028</v>
       </c>
     </row>
@@ -2606,6 +2450,7 @@
       </c>
     </row>
     <row r="13" spans="1:85" x14ac:dyDescent="0.2">
+      <c r="G13" s="3"/>
       <c r="Q13" s="4"/>
     </row>
     <row r="16" spans="1:85" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Tarik ha pagato 50€
</commit_message>
<xml_diff>
--- a/Netflix.xlsx
+++ b/Netflix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Netflix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1AEDC3-4171-4464-A89D-59B00C98DE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427C0BB9-471A-4799-A389-BDE63B37C6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
     <t>Rida</t>
   </si>
@@ -429,7 +429,7 @@
   <dimension ref="A1:CG16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1354,60 +1354,47 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
-        <f>ROUND(N8/N9,  1)</f>
-        <v>3.6</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ref="C4:BN4" si="6">ROUND(O8/O9,  1)</f>
-        <v>3.6</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="6"/>
-        <v>3.6</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="6"/>
-        <v>3.6</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="6"/>
-        <v>3.6</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" si="6"/>
-        <v>3.6</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="I4" s="1">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="J4" s="1">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="K4" s="1">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="L4" s="1">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="M4" s="1">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
+        <v>3.1</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="C4:BN4" si="6">ROUND(AA8/AA9,  1)</f>
         <v>4.5</v>
       </c>
       <c r="P4" s="1">
@@ -1651,287 +1638,287 @@
         <v>2023</v>
       </c>
       <c r="C5" s="1">
-        <f>IF(N1=12,B5+1,B5)</f>
+        <f t="shared" ref="C5:AH5" si="8">IF(N1=12,B5+1,B5)</f>
         <v>2023</v>
       </c>
       <c r="D5" s="1">
-        <f>IF(O1=12,C5+1,C5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="E5" s="1">
-        <f>IF(P1=12,D5+1,D5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="F5" s="1">
-        <f>IF(Q1=12,E5+1,E5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="G5" s="1">
-        <f>IF(R1=12,F5+1,F5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="H5" s="1">
-        <f>IF(S1=12,G5+1,G5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="I5" s="1">
-        <f>IF(T1=12,H5+1,H5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="J5" s="1">
-        <f>IF(U1=12,I5+1,I5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="K5" s="1">
-        <f>IF(V1=12,J5+1,J5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="L5" s="1">
-        <f>IF(W1=12,K5+1,K5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="M5" s="1">
-        <f>IF(X1=12,L5+1,L5)</f>
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="N5" s="1">
-        <f>IF(Y1=12,M5+1,M5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="O5" s="1">
-        <f>IF(Z1=12,N5+1,N5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="P5" s="1">
-        <f>IF(AA1=12,O5+1,O5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="Q5" s="1">
-        <f>IF(AB1=12,P5+1,P5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="R5" s="1">
-        <f>IF(AC1=12,Q5+1,Q5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="S5" s="1">
-        <f>IF(AD1=12,R5+1,R5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="T5" s="1">
-        <f>IF(AE1=12,S5+1,S5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="U5" s="1">
-        <f>IF(AF1=12,T5+1,T5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="V5" s="1">
-        <f>IF(AG1=12,U5+1,U5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="W5" s="1">
-        <f>IF(AH1=12,V5+1,V5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="X5" s="1">
-        <f>IF(AI1=12,W5+1,W5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="Y5" s="1">
-        <f>IF(AJ1=12,X5+1,X5)</f>
+        <f t="shared" si="8"/>
         <v>2024</v>
       </c>
       <c r="Z5" s="1">
-        <f>IF(AK1=12,Y5+1,Y5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AA5" s="1">
-        <f>IF(AL1=12,Z5+1,Z5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AB5" s="1">
-        <f>IF(AM1=12,AA5+1,AA5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AC5" s="1">
-        <f>IF(AN1=12,AB5+1,AB5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AD5" s="1">
-        <f>IF(AO1=12,AC5+1,AC5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AE5" s="1">
-        <f>IF(AP1=12,AD5+1,AD5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AF5" s="1">
-        <f>IF(AQ1=12,AE5+1,AE5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AG5" s="1">
-        <f>IF(AR1=12,AF5+1,AF5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AH5" s="1">
-        <f>IF(AS1=12,AG5+1,AG5)</f>
+        <f t="shared" si="8"/>
         <v>2025</v>
       </c>
       <c r="AI5" s="1">
-        <f>IF(AT1=12,AH5+1,AH5)</f>
+        <f t="shared" ref="AI5:BN5" si="9">IF(AT1=12,AH5+1,AH5)</f>
         <v>2025</v>
       </c>
       <c r="AJ5" s="1">
-        <f>IF(AU1=12,AI5+1,AI5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AK5" s="1">
-        <f>IF(AV1=12,AJ5+1,AJ5)</f>
+        <f t="shared" si="9"/>
         <v>2025</v>
       </c>
       <c r="AL5" s="1">
-        <f>IF(AW1=12,AK5+1,AK5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AM5" s="1">
-        <f>IF(AX1=12,AL5+1,AL5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AN5" s="1">
-        <f>IF(AY1=12,AM5+1,AM5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AO5" s="1">
-        <f>IF(AZ1=12,AN5+1,AN5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AP5" s="1">
-        <f>IF(BA1=12,AO5+1,AO5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AQ5" s="1">
-        <f>IF(BB1=12,AP5+1,AP5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AR5" s="1">
-        <f>IF(BC1=12,AQ5+1,AQ5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AS5" s="1">
-        <f>IF(BD1=12,AR5+1,AR5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AT5" s="1">
-        <f>IF(BE1=12,AS5+1,AS5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AU5" s="1">
-        <f>IF(BF1=12,AT5+1,AT5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AV5" s="1">
-        <f>IF(BG1=12,AU5+1,AU5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AW5" s="1">
-        <f>IF(BH1=12,AV5+1,AV5)</f>
+        <f t="shared" si="9"/>
         <v>2026</v>
       </c>
       <c r="AX5" s="1">
-        <f>IF(BI1=12,AW5+1,AW5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="AY5" s="1">
-        <f>IF(BJ1=12,AX5+1,AX5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="AZ5" s="1">
-        <f>IF(BK1=12,AY5+1,AY5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BA5" s="1">
-        <f>IF(BL1=12,AZ5+1,AZ5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BB5" s="1">
-        <f>IF(BM1=12,BA5+1,BA5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BC5" s="1">
-        <f>IF(BN1=12,BB5+1,BB5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BD5" s="1">
-        <f>IF(BO1=12,BC5+1,BC5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BE5" s="1">
-        <f>IF(BP1=12,BD5+1,BD5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BF5" s="1">
-        <f>IF(BQ1=12,BE5+1,BE5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BG5" s="1">
-        <f>IF(BR1=12,BF5+1,BF5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BH5" s="1">
-        <f>IF(BS1=12,BG5+1,BG5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BI5" s="1">
-        <f>IF(BT1=12,BH5+1,BH5)</f>
+        <f t="shared" si="9"/>
         <v>2027</v>
       </c>
       <c r="BJ5" s="1">
-        <f>IF(BU1=12,BI5+1,BI5)</f>
+        <f t="shared" si="9"/>
         <v>2028</v>
       </c>
       <c r="BK5" s="1">
-        <f>IF(BV1=12,BJ5+1,BJ5)</f>
+        <f t="shared" si="9"/>
         <v>2028</v>
       </c>
       <c r="BL5" s="1">
-        <f>IF(BW1=12,BK5+1,BK5)</f>
+        <f t="shared" si="9"/>
         <v>2028</v>
       </c>
       <c r="BM5" s="1">
-        <f>IF(BX1=12,BL5+1,BL5)</f>
+        <f t="shared" si="9"/>
         <v>2028</v>
       </c>
       <c r="BN5" s="1">
-        <f>IF(BY1=12,BM5+1,BM5)</f>
+        <f t="shared" si="9"/>
         <v>2028</v>
       </c>
       <c r="BO5" s="1">
-        <f>IF(BZ1=12,BN5+1,BN5)</f>
+        <f t="shared" ref="BO5:CT5" si="10">IF(BZ1=12,BN5+1,BN5)</f>
         <v>2028</v>
       </c>
       <c r="BP5" s="1">
-        <f>IF(CA1=12,BO5+1,BO5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BQ5" s="1">
-        <f>IF(CB1=12,BP5+1,BP5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BR5" s="1">
-        <f>IF(CC1=12,BQ5+1,BQ5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BS5" s="1">
-        <f>IF(CD1=12,BR5+1,BR5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BT5" s="1">
-        <f>IF(CE1=12,BS5+1,BS5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
       <c r="BU5" s="1">
-        <f>IF(CF1=12,BT5+1,BT5)</f>
+        <f t="shared" si="10"/>
         <v>2028</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tarik ha pagato 100 euro il 3/11/2025
</commit_message>
<xml_diff>
--- a/Netflix.xlsx
+++ b/Netflix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Netflix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDDB996-C9D7-413D-8FBA-698BE2CC5362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980F2DF4-1DAA-472E-A0A6-F286300F78F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="9">
   <si>
     <t>MESE</t>
   </si>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1239,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="AI3" s="2">
-        <f t="shared" ref="AH3:BM3" si="4">ROUND(AU8/AU9,  1)</f>
+        <f t="shared" ref="AI3:BM3" si="4">ROUND(AU8/AU9,  1)</f>
         <v>5</v>
       </c>
       <c r="AJ3" s="2">
@@ -1363,7 +1363,7 @@
         <v>5</v>
       </c>
       <c r="BN3" s="2">
-        <f t="shared" ref="BN3:CS3" si="5">ROUND(BZ8/BZ9,  1)</f>
+        <f t="shared" ref="BN3:BU3" si="5">ROUND(BZ8/BZ9,  1)</f>
         <v>5</v>
       </c>
       <c r="BO3" s="2">
@@ -1435,71 +1435,56 @@
       <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="2">
-        <v>3.1</v>
-      </c>
-      <c r="O4" s="2">
-        <f t="shared" ref="O4:AT4" si="6">ROUND(AA8/AA9,  1)</f>
-        <v>4.5</v>
-      </c>
-      <c r="P4" s="2">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="Q4" s="2">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="R4" s="2">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="S4" s="2">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="T4" s="2">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="U4" s="2">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="V4" s="2">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="W4" s="2">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="X4" s="2">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Y4" s="2">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="Z4" s="2">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="AA4" s="2">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="AB4" s="2">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="AC4" s="2">
-        <f t="shared" si="6"/>
-        <v>5</v>
+      <c r="N4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="AD4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="O4:AT4" si="6">ROUND(AP8/AP9,  1)</f>
         <v>5</v>
       </c>
       <c r="AE4" s="2">
@@ -1567,7 +1552,7 @@
         <v>5</v>
       </c>
       <c r="AU4" s="2">
-        <f t="shared" ref="AU4:BZ4" si="7">ROUND(BG8/BG9,  1)</f>
+        <f t="shared" ref="AU4:BU4" si="7">ROUND(BG8/BG9,  1)</f>
         <v>5</v>
       </c>
       <c r="AV4" s="2">
@@ -1939,7 +1924,7 @@
         <v>2028</v>
       </c>
       <c r="BO5" s="2">
-        <f t="shared" ref="BO5:CT5" si="10">IF(BZ1=12,BN5+1,BN5)</f>
+        <f t="shared" ref="BO5:BU5" si="10">IF(BZ1=12,BN5+1,BN5)</f>
         <v>2028</v>
       </c>
       <c r="BP5" s="2">
@@ -2512,7 +2497,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rida ha pagato 200 euro il 25/12/2025, 2025 pagato, resto in basta per eventuali cambiamenti di prezzo
</commit_message>
<xml_diff>
--- a/Netflix.xlsx
+++ b/Netflix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Netflix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980F2DF4-1DAA-472E-A0A6-F286300F78F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8007BA0-1FB3-4E8D-A9F4-142CD0F9E9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="9">
   <si>
     <t>MESE</t>
   </si>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1131,7 +1131,55 @@
         <v>5</v>
       </c>
       <c r="BU2" s="2">
-        <f t="shared" si="3"/>
+        <f>ROUND(BU8/BU9,  1)</f>
+        <v>5</v>
+      </c>
+      <c r="BV2" s="2">
+        <f t="shared" ref="BV2:CG2" si="4">ROUND(BV8/BV9,  1)</f>
+        <v>5</v>
+      </c>
+      <c r="BW2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="BX2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="BY2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="BZ2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="CA2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="CB2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="CC2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="CD2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="CE2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="CF2" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="CG2" s="2">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -1238,160 +1286,205 @@
       <c r="AH3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AI3" s="2">
-        <f t="shared" ref="AI3:BM3" si="4">ROUND(AU8/AU9,  1)</f>
-        <v>5</v>
-      </c>
-      <c r="AJ3" s="2">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="AK3" s="2">
-        <f t="shared" si="4"/>
-        <v>5</v>
+      <c r="AI3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="AL3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AI3:BM3" si="5">ROUND(AX8/AX9,  1)</f>
         <v>5</v>
       </c>
       <c r="AM3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AN3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AO3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AP3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AQ3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AR3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AS3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AT3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AU3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AV3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AW3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AX3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AY3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AZ3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BA3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BB3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BC3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BD3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BE3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BF3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BG3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BH3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BI3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BJ3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BK3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BL3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BM3" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="BN3" s="2">
-        <f t="shared" ref="BN3:BU3" si="5">ROUND(BZ8/BZ9,  1)</f>
+        <f t="shared" ref="BN3:BU3" si="6">ROUND(BZ8/BZ9,  1)</f>
         <v>5</v>
       </c>
       <c r="BO3" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="BP3" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="BQ3" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="BR3" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="BS3" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="BT3" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="BU3" s="2">
-        <f t="shared" si="5"/>
+        <f>ROUND(BU8/BU9,  1)</f>
+        <v>5</v>
+      </c>
+      <c r="BV3" s="2">
+        <f t="shared" ref="BV3:CG3" si="7">ROUND(BV8/BV9,  1)</f>
+        <v>5</v>
+      </c>
+      <c r="BW3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="BX3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="BY3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="BZ3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="CA3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="CB3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="CC3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="CD3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="CE3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="CF3" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="CG3" s="2">
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -1484,179 +1577,227 @@
         <v>2</v>
       </c>
       <c r="AD4" s="2">
-        <f t="shared" ref="O4:AT4" si="6">ROUND(AP8/AP9,  1)</f>
+        <f t="shared" ref="AD4:AT4" si="8">ROUND(AP8/AP9,  1)</f>
         <v>5</v>
       </c>
       <c r="AE4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AF4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AG4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AH4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AI4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AJ4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AK4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AL4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AM4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AN4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AO4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AP4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AQ4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AR4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AS4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AT4" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AU4" s="2">
-        <f t="shared" ref="AU4:BU4" si="7">ROUND(BG8/BG9,  1)</f>
+        <f t="shared" ref="AU4:BU4" si="9">ROUND(BG8/BG9,  1)</f>
         <v>5</v>
       </c>
       <c r="AV4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AW4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AX4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AY4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AZ4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BA4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BB4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BC4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BD4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BE4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BF4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BG4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BH4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BI4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BJ4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BK4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BL4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BM4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BN4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BO4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BP4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BQ4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BR4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BS4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BT4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="BU4" s="2">
-        <f t="shared" si="7"/>
+        <f>ROUND(BU8/BU9,  1)</f>
+        <v>5</v>
+      </c>
+      <c r="BV4" s="2">
+        <f t="shared" ref="BV4:CG4" si="10">ROUND(BV8/BV9,  1)</f>
+        <v>5</v>
+      </c>
+      <c r="BW4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="BX4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="BY4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="BZ4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="CA4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="CB4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="CC4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="CD4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="CE4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="CF4" s="2">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="CG4" s="2">
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
     </row>
@@ -1668,288 +1809,336 @@
         <v>2023</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:AH5" si="8">IF(N1=12,B5+1,B5)</f>
+        <f t="shared" ref="C5:AH5" si="11">IF(N1=12,B5+1,B5)</f>
         <v>2023</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="P5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="Q5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="R5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="S5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="T5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="U5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="V5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="W5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="X5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="Y5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
       <c r="Z5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AA5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AB5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AC5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AD5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AE5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AF5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AG5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AH5" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2025</v>
       </c>
       <c r="AI5" s="2">
-        <f t="shared" ref="AI5:BN5" si="9">IF(AT1=12,AH5+1,AH5)</f>
+        <f t="shared" ref="AI5:BN5" si="12">IF(AT1=12,AH5+1,AH5)</f>
         <v>2025</v>
       </c>
       <c r="AJ5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2025</v>
       </c>
       <c r="AK5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2025</v>
       </c>
       <c r="AL5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AM5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AN5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AO5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AP5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AQ5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AR5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AS5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AT5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AU5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AV5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AW5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2026</v>
       </c>
       <c r="AX5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="AY5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="AZ5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BA5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BB5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BC5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BD5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BE5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BF5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BG5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BH5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BI5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2027</v>
       </c>
       <c r="BJ5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2028</v>
       </c>
       <c r="BK5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2028</v>
       </c>
       <c r="BL5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2028</v>
       </c>
       <c r="BM5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2028</v>
       </c>
       <c r="BN5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2028</v>
       </c>
       <c r="BO5" s="2">
-        <f t="shared" ref="BO5:BU5" si="10">IF(BZ1=12,BN5+1,BN5)</f>
+        <f t="shared" ref="BO5:BU5" si="13">IF(BZ1=12,BN5+1,BN5)</f>
         <v>2028</v>
       </c>
       <c r="BP5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2028</v>
       </c>
       <c r="BQ5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2028</v>
       </c>
       <c r="BR5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2028</v>
       </c>
       <c r="BS5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2028</v>
       </c>
       <c r="BT5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2028</v>
       </c>
       <c r="BU5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2028</v>
+      </c>
+      <c r="BV5" s="2">
+        <f t="shared" ref="BV5" si="14">IF(CG1=12,BU5+1,BU5)</f>
+        <v>2029</v>
+      </c>
+      <c r="BW5" s="2">
+        <f t="shared" ref="BW5" si="15">IF(CH1=12,BV5+1,BV5)</f>
+        <v>2029</v>
+      </c>
+      <c r="BX5" s="2">
+        <f t="shared" ref="BX5" si="16">IF(CI1=12,BW5+1,BW5)</f>
+        <v>2029</v>
+      </c>
+      <c r="BY5" s="2">
+        <f t="shared" ref="BY5" si="17">IF(CJ1=12,BX5+1,BX5)</f>
+        <v>2029</v>
+      </c>
+      <c r="BZ5" s="2">
+        <f t="shared" ref="BZ5" si="18">IF(CK1=12,BY5+1,BY5)</f>
+        <v>2029</v>
+      </c>
+      <c r="CA5" s="2">
+        <f t="shared" ref="CA5" si="19">IF(CL1=12,BZ5+1,BZ5)</f>
+        <v>2029</v>
+      </c>
+      <c r="CB5" s="2">
+        <f t="shared" ref="CB5" si="20">IF(CM1=12,CA5+1,CA5)</f>
+        <v>2029</v>
+      </c>
+      <c r="CC5" s="2">
+        <f t="shared" ref="CC5" si="21">IF(CN1=12,CB5+1,CB5)</f>
+        <v>2029</v>
+      </c>
+      <c r="CD5" s="2">
+        <f t="shared" ref="CD5" si="22">IF(CO1=12,CC5+1,CC5)</f>
+        <v>2029</v>
+      </c>
+      <c r="CE5" s="2">
+        <f t="shared" ref="CE5" si="23">IF(CP1=12,CD5+1,CD5)</f>
+        <v>2029</v>
+      </c>
+      <c r="CF5" s="2">
+        <f t="shared" ref="CF5" si="24">IF(CQ1=12,CE5+1,CE5)</f>
+        <v>2029</v>
+      </c>
+      <c r="CG5" s="2">
+        <f t="shared" ref="CG5" si="25">IF(CR1=12,CF5+1,CF5)</f>
+        <v>2029</v>
       </c>
     </row>
     <row r="8" spans="1:85" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2489,7 +2678,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="1">
-        <v>0.9</v>
+        <v>185.9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>